<commit_message>
Criação de notebook com todas as respostas
</commit_message>
<xml_diff>
--- a/arquivos/respostas-questionario.xlsx
+++ b/arquivos/respostas-questionario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\demet\git\ppca-taes\arquivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{261D8556-620B-4778-BF4F-387F10ABCCEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED786689-1762-4781-B3D0-4C0997D5FCC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-18030" yWindow="240" windowWidth="14400" windowHeight="7335" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Respostas ao formulário 1" sheetId="1" r:id="rId1"/>
@@ -365,11 +365,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:V18"/>
+  <dimension ref="A1:V21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17:V18"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A19" sqref="A19:V21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -377,7 +377,7 @@
     <col min="1" max="22" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -427,7 +427,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>44903.465021886572</v>
       </c>
@@ -477,7 +477,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>44903.470373229167</v>
       </c>
@@ -527,7 +527,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>44903.475477592598</v>
       </c>
@@ -577,7 +577,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>44903.485396851851</v>
       </c>
@@ -627,7 +627,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>44903.49244850695</v>
       </c>
@@ -677,7 +677,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>44903.556095</v>
       </c>
@@ -727,7 +727,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>44903.591057418977</v>
       </c>
@@ -777,7 +777,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>44903.630790914351</v>
       </c>
@@ -827,7 +827,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>44903.633577754634</v>
       </c>
@@ -877,7 +877,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>44903.807695740739</v>
       </c>
@@ -927,7 +927,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>44904.364620729168</v>
       </c>
@@ -977,7 +977,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>44904.440244583333</v>
       </c>
@@ -1027,7 +1027,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>44904.471218252314</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>44906.276969247687</v>
       </c>
@@ -1289,7 +1289,176 @@
       <c r="U18" s="5"/>
       <c r="V18" s="5"/>
     </row>
+    <row r="19" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>44911.447951388887</v>
+      </c>
+      <c r="B19" s="4">
+        <v>3</v>
+      </c>
+      <c r="C19" s="4">
+        <v>4</v>
+      </c>
+      <c r="D19" s="4">
+        <v>3</v>
+      </c>
+      <c r="E19" s="4">
+        <v>3</v>
+      </c>
+      <c r="F19" s="4">
+        <v>4</v>
+      </c>
+      <c r="G19" s="4">
+        <v>2</v>
+      </c>
+      <c r="H19" s="4">
+        <v>3</v>
+      </c>
+      <c r="I19" s="4">
+        <v>2</v>
+      </c>
+      <c r="J19" s="4">
+        <v>3</v>
+      </c>
+      <c r="K19" s="4">
+        <v>4</v>
+      </c>
+      <c r="L19" s="4">
+        <v>2</v>
+      </c>
+      <c r="M19" s="4">
+        <v>3</v>
+      </c>
+      <c r="N19" s="4">
+        <v>3</v>
+      </c>
+      <c r="O19" s="4">
+        <v>4</v>
+      </c>
+      <c r="P19" s="4">
+        <v>4</v>
+      </c>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+      <c r="S19" s="5"/>
+      <c r="T19" s="5"/>
+      <c r="U19" s="5"/>
+      <c r="V19" s="5"/>
+    </row>
+    <row r="20" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>44911.484768518516</v>
+      </c>
+      <c r="B20" s="4">
+        <v>5</v>
+      </c>
+      <c r="C20" s="4">
+        <v>5</v>
+      </c>
+      <c r="D20" s="4">
+        <v>5</v>
+      </c>
+      <c r="E20" s="4">
+        <v>1</v>
+      </c>
+      <c r="F20" s="4">
+        <v>5</v>
+      </c>
+      <c r="G20" s="4">
+        <v>1</v>
+      </c>
+      <c r="H20" s="4">
+        <v>5</v>
+      </c>
+      <c r="I20" s="4">
+        <v>1</v>
+      </c>
+      <c r="J20" s="4">
+        <v>1</v>
+      </c>
+      <c r="K20" s="4">
+        <v>5</v>
+      </c>
+      <c r="L20" s="4">
+        <v>1</v>
+      </c>
+      <c r="M20" s="4">
+        <v>4</v>
+      </c>
+      <c r="N20" s="4">
+        <v>1</v>
+      </c>
+      <c r="O20" s="4">
+        <v>5</v>
+      </c>
+      <c r="P20" s="4">
+        <v>5</v>
+      </c>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="5"/>
+      <c r="S20" s="5"/>
+      <c r="T20" s="5"/>
+      <c r="U20" s="5"/>
+      <c r="V20" s="5"/>
+    </row>
+    <row r="21" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>44914.534548611111</v>
+      </c>
+      <c r="B21" s="4">
+        <v>5</v>
+      </c>
+      <c r="C21" s="4">
+        <v>5</v>
+      </c>
+      <c r="D21" s="4">
+        <v>5</v>
+      </c>
+      <c r="E21" s="4">
+        <v>1</v>
+      </c>
+      <c r="F21" s="4">
+        <v>5</v>
+      </c>
+      <c r="G21" s="4">
+        <v>1</v>
+      </c>
+      <c r="H21" s="4">
+        <v>5</v>
+      </c>
+      <c r="I21" s="4">
+        <v>1</v>
+      </c>
+      <c r="J21" s="4">
+        <v>1</v>
+      </c>
+      <c r="K21" s="4">
+        <v>5</v>
+      </c>
+      <c r="L21" s="4">
+        <v>1</v>
+      </c>
+      <c r="M21" s="4">
+        <v>5</v>
+      </c>
+      <c r="N21" s="4">
+        <v>1</v>
+      </c>
+      <c r="O21" s="4">
+        <v>5</v>
+      </c>
+      <c r="P21" s="4">
+        <v>5</v>
+      </c>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5"/>
+      <c r="S21" s="5"/>
+      <c r="T21" s="5"/>
+      <c r="U21" s="5"/>
+      <c r="V21" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>